<commit_message>
flowchart test cases and reflection
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eileen Martinez\PycharmProjects\cs151-lab7-antonio_oreoluwa_jalen_lab07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF27D802-FB15-694F-BF0B-8F3CB3EC9386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6EE487-5CAE-4F3F-8419-5AA529C229D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="5960" yWindow="0" windowWidth="16690" windowHeight="15130" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>&lt;-- final overall cost</t>
   </si>
@@ -58,6 +49,15 @@
   </si>
   <si>
     <t>cost/sqft</t>
+  </si>
+  <si>
+    <t>hardwood</t>
+  </si>
+  <si>
+    <t>carpet</t>
+  </si>
+  <si>
+    <t>tile</t>
   </si>
 </sst>
 </file>
@@ -212,11 +212,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -572,10 +572,10 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -585,22 +585,22 @@
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -614,53 +614,107 @@
         <v>1</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1.39</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>152.9</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3.99</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>335.16</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.99</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>383.04</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>299.39999999999998</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3">
+        <v>404.19</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>1504.69</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>